<commit_message>
Fix database, update mwb file
</commit_message>
<xml_diff>
--- a/doc/backend/db/TRN-MiniBlog_DatabaseDesign_UayLe.xlsx
+++ b/doc/backend/db/TRN-MiniBlog_DatabaseDesign_UayLe.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25120" windowHeight="15600" tabRatio="818" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25020" windowHeight="15600" tabRatio="818" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="11" r:id="rId1"/>
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="188">
   <si>
     <t>No</t>
   </si>
@@ -639,9 +639,6 @@
     <t>author_id</t>
   </si>
   <si>
-    <t>LONGTEXT</t>
-  </si>
-  <si>
     <t>VARCHAR(150)</t>
   </si>
   <si>
@@ -711,10 +708,16 @@
     <t>access_key</t>
   </si>
   <si>
-    <t>YES</t>
-  </si>
-  <si>
     <t>hash md5</t>
+  </si>
+  <si>
+    <t>VARCHAR(3000)</t>
+  </si>
+  <si>
+    <t>VARCHAR(72)</t>
+  </si>
+  <si>
+    <t>23/01/2015</t>
   </si>
 </sst>
 </file>
@@ -1810,7 +1813,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="482">
+  <cellStyleXfs count="483">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1830,6 +1833,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3715,6 +3721,9 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3911,11 +3920,8 @@
     <xf numFmtId="49" fontId="22" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="482">
+  <cellStyles count="483">
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
@@ -4390,6 +4396,7 @@
     <cellStyle name="Followed Hyperlink" xfId="479" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="480" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="481" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="482" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="ハイパーリンク 2" xfId="4"/>
@@ -5643,29 +5650,29 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
-      <c r="O13" s="167"/>
-      <c r="P13" s="167"/>
-      <c r="Q13" s="167"/>
-      <c r="R13" s="167"/>
-      <c r="S13" s="167"/>
-      <c r="T13" s="167"/>
-      <c r="U13" s="167"/>
-      <c r="V13" s="167"/>
-      <c r="W13" s="167"/>
-      <c r="X13" s="167"/>
-      <c r="Y13" s="167"/>
-      <c r="Z13" s="167"/>
-      <c r="AA13" s="167"/>
-      <c r="AB13" s="167"/>
-      <c r="AC13" s="167"/>
-      <c r="AD13" s="167"/>
-      <c r="AE13" s="167"/>
-      <c r="AF13" s="167"/>
-      <c r="AG13" s="167"/>
-      <c r="AH13" s="167"/>
-      <c r="AI13" s="167"/>
-      <c r="AJ13" s="167"/>
-      <c r="AK13" s="167"/>
+      <c r="O13" s="168"/>
+      <c r="P13" s="168"/>
+      <c r="Q13" s="168"/>
+      <c r="R13" s="168"/>
+      <c r="S13" s="168"/>
+      <c r="T13" s="168"/>
+      <c r="U13" s="168"/>
+      <c r="V13" s="168"/>
+      <c r="W13" s="168"/>
+      <c r="X13" s="168"/>
+      <c r="Y13" s="168"/>
+      <c r="Z13" s="168"/>
+      <c r="AA13" s="168"/>
+      <c r="AB13" s="168"/>
+      <c r="AC13" s="168"/>
+      <c r="AD13" s="168"/>
+      <c r="AE13" s="168"/>
+      <c r="AF13" s="168"/>
+      <c r="AG13" s="168"/>
+      <c r="AH13" s="168"/>
+      <c r="AI13" s="168"/>
+      <c r="AJ13" s="168"/>
+      <c r="AK13" s="168"/>
       <c r="AL13" s="4"/>
       <c r="AM13" s="4"/>
       <c r="AN13" s="4"/>
@@ -5697,29 +5704,29 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
-      <c r="O14" s="167"/>
-      <c r="P14" s="167"/>
-      <c r="Q14" s="167"/>
-      <c r="R14" s="167"/>
-      <c r="S14" s="167"/>
-      <c r="T14" s="167"/>
-      <c r="U14" s="167"/>
-      <c r="V14" s="167"/>
-      <c r="W14" s="167"/>
-      <c r="X14" s="167"/>
-      <c r="Y14" s="167"/>
-      <c r="Z14" s="167"/>
-      <c r="AA14" s="167"/>
-      <c r="AB14" s="167"/>
-      <c r="AC14" s="167"/>
-      <c r="AD14" s="167"/>
-      <c r="AE14" s="167"/>
-      <c r="AF14" s="167"/>
-      <c r="AG14" s="167"/>
-      <c r="AH14" s="167"/>
-      <c r="AI14" s="167"/>
-      <c r="AJ14" s="167"/>
-      <c r="AK14" s="167"/>
+      <c r="O14" s="168"/>
+      <c r="P14" s="168"/>
+      <c r="Q14" s="168"/>
+      <c r="R14" s="168"/>
+      <c r="S14" s="168"/>
+      <c r="T14" s="168"/>
+      <c r="U14" s="168"/>
+      <c r="V14" s="168"/>
+      <c r="W14" s="168"/>
+      <c r="X14" s="168"/>
+      <c r="Y14" s="168"/>
+      <c r="Z14" s="168"/>
+      <c r="AA14" s="168"/>
+      <c r="AB14" s="168"/>
+      <c r="AC14" s="168"/>
+      <c r="AD14" s="168"/>
+      <c r="AE14" s="168"/>
+      <c r="AF14" s="168"/>
+      <c r="AG14" s="168"/>
+      <c r="AH14" s="168"/>
+      <c r="AI14" s="168"/>
+      <c r="AJ14" s="168"/>
+      <c r="AK14" s="168"/>
       <c r="AL14" s="4"/>
       <c r="AM14" s="4"/>
       <c r="AN14" s="4"/>
@@ -5747,43 +5754,43 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="168" t="s">
+      <c r="K15" s="169" t="s">
         <v>117</v>
       </c>
-      <c r="L15" s="168"/>
-      <c r="M15" s="168"/>
-      <c r="N15" s="168"/>
-      <c r="O15" s="168"/>
-      <c r="P15" s="168"/>
-      <c r="Q15" s="168"/>
-      <c r="R15" s="168"/>
-      <c r="S15" s="168"/>
-      <c r="T15" s="168"/>
-      <c r="U15" s="168"/>
-      <c r="V15" s="168"/>
-      <c r="W15" s="168"/>
-      <c r="X15" s="168"/>
-      <c r="Y15" s="168"/>
-      <c r="Z15" s="168"/>
-      <c r="AA15" s="168"/>
-      <c r="AB15" s="168"/>
-      <c r="AC15" s="168"/>
-      <c r="AD15" s="168"/>
-      <c r="AE15" s="168"/>
-      <c r="AF15" s="168"/>
-      <c r="AG15" s="168"/>
-      <c r="AH15" s="168"/>
-      <c r="AI15" s="168"/>
-      <c r="AJ15" s="168"/>
-      <c r="AK15" s="168"/>
-      <c r="AL15" s="168"/>
-      <c r="AM15" s="168"/>
-      <c r="AN15" s="168"/>
-      <c r="AO15" s="168"/>
-      <c r="AP15" s="168"/>
-      <c r="AQ15" s="168"/>
-      <c r="AR15" s="168"/>
-      <c r="AS15" s="168"/>
+      <c r="L15" s="169"/>
+      <c r="M15" s="169"/>
+      <c r="N15" s="169"/>
+      <c r="O15" s="169"/>
+      <c r="P15" s="169"/>
+      <c r="Q15" s="169"/>
+      <c r="R15" s="169"/>
+      <c r="S15" s="169"/>
+      <c r="T15" s="169"/>
+      <c r="U15" s="169"/>
+      <c r="V15" s="169"/>
+      <c r="W15" s="169"/>
+      <c r="X15" s="169"/>
+      <c r="Y15" s="169"/>
+      <c r="Z15" s="169"/>
+      <c r="AA15" s="169"/>
+      <c r="AB15" s="169"/>
+      <c r="AC15" s="169"/>
+      <c r="AD15" s="169"/>
+      <c r="AE15" s="169"/>
+      <c r="AF15" s="169"/>
+      <c r="AG15" s="169"/>
+      <c r="AH15" s="169"/>
+      <c r="AI15" s="169"/>
+      <c r="AJ15" s="169"/>
+      <c r="AK15" s="169"/>
+      <c r="AL15" s="169"/>
+      <c r="AM15" s="169"/>
+      <c r="AN15" s="169"/>
+      <c r="AO15" s="169"/>
+      <c r="AP15" s="169"/>
+      <c r="AQ15" s="169"/>
+      <c r="AR15" s="169"/>
+      <c r="AS15" s="169"/>
       <c r="AT15" s="4"/>
       <c r="AU15" s="4"/>
       <c r="AV15" s="4"/>
@@ -5803,41 +5810,41 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="168"/>
-      <c r="L16" s="168"/>
-      <c r="M16" s="168"/>
-      <c r="N16" s="168"/>
-      <c r="O16" s="168"/>
-      <c r="P16" s="168"/>
-      <c r="Q16" s="168"/>
-      <c r="R16" s="168"/>
-      <c r="S16" s="168"/>
-      <c r="T16" s="168"/>
-      <c r="U16" s="168"/>
-      <c r="V16" s="168"/>
-      <c r="W16" s="168"/>
-      <c r="X16" s="168"/>
-      <c r="Y16" s="168"/>
-      <c r="Z16" s="168"/>
-      <c r="AA16" s="168"/>
-      <c r="AB16" s="168"/>
-      <c r="AC16" s="168"/>
-      <c r="AD16" s="168"/>
-      <c r="AE16" s="168"/>
-      <c r="AF16" s="168"/>
-      <c r="AG16" s="168"/>
-      <c r="AH16" s="168"/>
-      <c r="AI16" s="168"/>
-      <c r="AJ16" s="168"/>
-      <c r="AK16" s="168"/>
-      <c r="AL16" s="168"/>
-      <c r="AM16" s="168"/>
-      <c r="AN16" s="168"/>
-      <c r="AO16" s="168"/>
-      <c r="AP16" s="168"/>
-      <c r="AQ16" s="168"/>
-      <c r="AR16" s="168"/>
-      <c r="AS16" s="168"/>
+      <c r="K16" s="169"/>
+      <c r="L16" s="169"/>
+      <c r="M16" s="169"/>
+      <c r="N16" s="169"/>
+      <c r="O16" s="169"/>
+      <c r="P16" s="169"/>
+      <c r="Q16" s="169"/>
+      <c r="R16" s="169"/>
+      <c r="S16" s="169"/>
+      <c r="T16" s="169"/>
+      <c r="U16" s="169"/>
+      <c r="V16" s="169"/>
+      <c r="W16" s="169"/>
+      <c r="X16" s="169"/>
+      <c r="Y16" s="169"/>
+      <c r="Z16" s="169"/>
+      <c r="AA16" s="169"/>
+      <c r="AB16" s="169"/>
+      <c r="AC16" s="169"/>
+      <c r="AD16" s="169"/>
+      <c r="AE16" s="169"/>
+      <c r="AF16" s="169"/>
+      <c r="AG16" s="169"/>
+      <c r="AH16" s="169"/>
+      <c r="AI16" s="169"/>
+      <c r="AJ16" s="169"/>
+      <c r="AK16" s="169"/>
+      <c r="AL16" s="169"/>
+      <c r="AM16" s="169"/>
+      <c r="AN16" s="169"/>
+      <c r="AO16" s="169"/>
+      <c r="AP16" s="169"/>
+      <c r="AQ16" s="169"/>
+      <c r="AR16" s="169"/>
+      <c r="AS16" s="169"/>
       <c r="AT16" s="4"/>
       <c r="AU16" s="4"/>
       <c r="AV16" s="4"/>
@@ -6426,14 +6433,14 @@
       <c r="AK27" s="4"/>
       <c r="AL27" s="4"/>
       <c r="AM27" s="7"/>
-      <c r="AN27" s="169" t="s">
+      <c r="AN27" s="170" t="s">
         <v>120</v>
       </c>
-      <c r="AO27" s="169"/>
-      <c r="AP27" s="169"/>
-      <c r="AQ27" s="169"/>
-      <c r="AR27" s="169"/>
-      <c r="AS27" s="169"/>
+      <c r="AO27" s="170"/>
+      <c r="AP27" s="170"/>
+      <c r="AQ27" s="170"/>
+      <c r="AR27" s="170"/>
+      <c r="AS27" s="170"/>
       <c r="AT27" s="12"/>
       <c r="AU27" s="12"/>
       <c r="AV27" s="12"/>
@@ -6923,103 +6930,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="171" t="s">
+      <c r="C2" s="172" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="172"/>
+      <c r="D2" s="173"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="231" t="s">
+      <c r="F2" s="232" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="232"/>
+      <c r="G2" s="233"/>
     </row>
     <row r="3" spans="1:14" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="173"/>
-      <c r="D3" s="174"/>
+      <c r="C3" s="174"/>
+      <c r="D3" s="175"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="176" t="s">
+      <c r="F3" s="177" t="s">
         <v>104</v>
       </c>
-      <c r="G3" s="177"/>
+      <c r="G3" s="178"/>
     </row>
     <row r="4" spans="1:14" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="173" t="s">
+      <c r="C4" s="174" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="174"/>
+      <c r="D4" s="175"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="173"/>
-      <c r="G4" s="177"/>
+      <c r="F4" s="174"/>
+      <c r="G4" s="178"/>
     </row>
     <row r="5" spans="1:14" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="173" t="s">
+      <c r="C5" s="174" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="174"/>
+      <c r="D5" s="175"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="173"/>
-      <c r="G5" s="177"/>
+      <c r="F5" s="174"/>
+      <c r="G5" s="178"/>
     </row>
     <row r="6" spans="1:14" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="173" t="s">
+      <c r="C6" s="174" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="174"/>
+      <c r="D6" s="175"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="173"/>
-      <c r="G6" s="177"/>
+      <c r="F6" s="174"/>
+      <c r="G6" s="178"/>
     </row>
     <row r="7" spans="1:14" ht="13">
-      <c r="B7" s="182" t="s">
+      <c r="B7" s="183" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="183"/>
-      <c r="D7" s="183"/>
-      <c r="E7" s="183"/>
-      <c r="F7" s="183"/>
-      <c r="G7" s="184"/>
+      <c r="C7" s="184"/>
+      <c r="D7" s="184"/>
+      <c r="E7" s="184"/>
+      <c r="F7" s="184"/>
+      <c r="G7" s="185"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="185"/>
-      <c r="C8" s="186"/>
-      <c r="D8" s="186"/>
-      <c r="E8" s="186"/>
-      <c r="F8" s="186"/>
-      <c r="G8" s="187"/>
+      <c r="B8" s="186"/>
+      <c r="C8" s="187"/>
+      <c r="D8" s="187"/>
+      <c r="E8" s="187"/>
+      <c r="F8" s="187"/>
+      <c r="G8" s="188"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="188"/>
-      <c r="C9" s="186"/>
-      <c r="D9" s="186"/>
-      <c r="E9" s="186"/>
-      <c r="F9" s="186"/>
-      <c r="G9" s="187"/>
+      <c r="B9" s="189"/>
+      <c r="C9" s="187"/>
+      <c r="D9" s="187"/>
+      <c r="E9" s="187"/>
+      <c r="F9" s="187"/>
+      <c r="G9" s="188"/>
     </row>
     <row r="10" spans="1:14" ht="12" thickBot="1">
-      <c r="B10" s="189"/>
-      <c r="C10" s="190"/>
-      <c r="D10" s="190"/>
-      <c r="E10" s="190"/>
-      <c r="F10" s="190"/>
-      <c r="G10" s="191"/>
+      <c r="B10" s="190"/>
+      <c r="C10" s="191"/>
+      <c r="D10" s="191"/>
+      <c r="E10" s="191"/>
+      <c r="F10" s="191"/>
+      <c r="G10" s="192"/>
     </row>
     <row r="11" spans="1:14">
       <c r="H11" s="87"/>
@@ -7235,10 +7242,10 @@
       <c r="B21" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="178" t="s">
+      <c r="C21" s="179" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="179"/>
+      <c r="D21" s="180"/>
       <c r="E21" s="34" t="s">
         <v>33</v>
       </c>
@@ -7262,10 +7269,10 @@
       <c r="B22" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="192" t="s">
+      <c r="C22" s="193" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="193"/>
+      <c r="D22" s="194"/>
       <c r="E22" s="46" t="s">
         <v>3</v>
       </c>
@@ -7285,10 +7292,10 @@
         <v>2</v>
       </c>
       <c r="B23" s="51"/>
-      <c r="C23" s="197" t="s">
+      <c r="C23" s="198" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="198"/>
+      <c r="D23" s="199"/>
       <c r="E23" s="52"/>
       <c r="F23" s="52" t="s">
         <v>3</v>
@@ -7306,10 +7313,10 @@
         <v>3</v>
       </c>
       <c r="B24" s="26"/>
-      <c r="C24" s="227" t="s">
+      <c r="C24" s="228" t="s">
         <v>69</v>
       </c>
-      <c r="D24" s="228"/>
+      <c r="D24" s="229"/>
       <c r="E24" s="45"/>
       <c r="F24" s="45" t="s">
         <v>3</v>
@@ -7348,14 +7355,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="180" t="s">
+      <c r="C27" s="181" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="181"/>
-      <c r="E27" s="180" t="s">
+      <c r="D27" s="182"/>
+      <c r="E27" s="181" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="194"/>
+      <c r="F27" s="195"/>
       <c r="G27" s="38" t="s">
         <v>38</v>
       </c>
@@ -7392,14 +7399,14 @@
       <c r="B30" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="180" t="s">
+      <c r="C30" s="181" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="181"/>
-      <c r="E30" s="180" t="s">
+      <c r="D30" s="182"/>
+      <c r="E30" s="181" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="194"/>
+      <c r="F30" s="195"/>
       <c r="G30" s="38" t="s">
         <v>39</v>
       </c>
@@ -7415,14 +7422,14 @@
         <v>1</v>
       </c>
       <c r="B31" s="51"/>
-      <c r="C31" s="192" t="s">
+      <c r="C31" s="193" t="s">
         <v>77</v>
       </c>
-      <c r="D31" s="193"/>
-      <c r="E31" s="197" t="s">
+      <c r="D31" s="194"/>
+      <c r="E31" s="198" t="s">
         <v>75</v>
       </c>
-      <c r="F31" s="198"/>
+      <c r="F31" s="199"/>
       <c r="G31" s="53" t="s">
         <v>77</v>
       </c>
@@ -7438,14 +7445,14 @@
         <v>2</v>
       </c>
       <c r="B32" s="26"/>
-      <c r="C32" s="229" t="s">
+      <c r="C32" s="230" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="230"/>
-      <c r="E32" s="207" t="s">
+      <c r="D32" s="231"/>
+      <c r="E32" s="208" t="s">
         <v>70</v>
       </c>
-      <c r="F32" s="208"/>
+      <c r="F32" s="209"/>
       <c r="G32" s="55" t="s">
         <v>52</v>
       </c>
@@ -7838,11 +7845,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12" thickBot="1">
-      <c r="A1" s="170" t="s">
+      <c r="A1" s="171" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
+      <c r="B1" s="171"/>
+      <c r="C1" s="171"/>
     </row>
     <row r="2" spans="1:3" ht="12" thickBot="1">
       <c r="A2" s="118" t="s">
@@ -7874,7 +7881,7 @@
       <c r="B4" s="123" t="s">
         <v>138</v>
       </c>
-      <c r="C4" s="233" t="s">
+      <c r="C4" s="167" t="s">
         <v>143</v>
       </c>
     </row>
@@ -7886,7 +7893,7 @@
       <c r="B5" s="123" t="s">
         <v>139</v>
       </c>
-      <c r="C5" s="233" t="s">
+      <c r="C5" s="167" t="s">
         <v>142</v>
       </c>
     </row>
@@ -7898,7 +7905,7 @@
       <c r="B6" s="123" t="s">
         <v>140</v>
       </c>
-      <c r="C6" s="233" t="s">
+      <c r="C6" s="167" t="s">
         <v>141</v>
       </c>
     </row>
@@ -8110,7 +8117,9 @@
   </sheetPr>
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:G7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
   <cols>
@@ -8139,103 +8148,105 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="171" t="s">
+      <c r="C2" s="172" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="172"/>
+      <c r="D2" s="173"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="171" t="s">
+      <c r="F2" s="172" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="175"/>
+      <c r="G2" s="176"/>
     </row>
     <row r="3" spans="1:17" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="173"/>
-      <c r="D3" s="174"/>
+      <c r="C3" s="174"/>
+      <c r="D3" s="175"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="176" t="s">
+      <c r="F3" s="177" t="s">
         <v>120</v>
       </c>
-      <c r="G3" s="177"/>
+      <c r="G3" s="178"/>
     </row>
     <row r="4" spans="1:17" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="173" t="s">
+      <c r="C4" s="174" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="174"/>
+      <c r="D4" s="175"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="173"/>
-      <c r="G4" s="177"/>
+      <c r="F4" s="174" t="s">
+        <v>187</v>
+      </c>
+      <c r="G4" s="178"/>
     </row>
     <row r="5" spans="1:17" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="173" t="s">
+      <c r="C5" s="174" t="s">
         <v>121</v>
       </c>
-      <c r="D5" s="174"/>
+      <c r="D5" s="175"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="173"/>
-      <c r="G5" s="177"/>
+      <c r="F5" s="174"/>
+      <c r="G5" s="178"/>
     </row>
     <row r="6" spans="1:17" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="173" t="s">
+      <c r="C6" s="174" t="s">
         <v>106</v>
       </c>
-      <c r="D6" s="174"/>
+      <c r="D6" s="175"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="173"/>
-      <c r="G6" s="177"/>
+      <c r="F6" s="174"/>
+      <c r="G6" s="178"/>
     </row>
     <row r="7" spans="1:17" ht="13">
-      <c r="B7" s="182" t="s">
+      <c r="B7" s="183" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="183"/>
-      <c r="D7" s="183"/>
-      <c r="E7" s="183"/>
-      <c r="F7" s="183"/>
-      <c r="G7" s="184"/>
+      <c r="C7" s="184"/>
+      <c r="D7" s="184"/>
+      <c r="E7" s="184"/>
+      <c r="F7" s="184"/>
+      <c r="G7" s="185"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="B8" s="185"/>
-      <c r="C8" s="186"/>
-      <c r="D8" s="186"/>
-      <c r="E8" s="186"/>
-      <c r="F8" s="186"/>
-      <c r="G8" s="187"/>
+      <c r="B8" s="186"/>
+      <c r="C8" s="187"/>
+      <c r="D8" s="187"/>
+      <c r="E8" s="187"/>
+      <c r="F8" s="187"/>
+      <c r="G8" s="188"/>
     </row>
     <row r="9" spans="1:17">
-      <c r="B9" s="188"/>
-      <c r="C9" s="186"/>
-      <c r="D9" s="186"/>
-      <c r="E9" s="186"/>
-      <c r="F9" s="186"/>
-      <c r="G9" s="187"/>
+      <c r="B9" s="189"/>
+      <c r="C9" s="187"/>
+      <c r="D9" s="187"/>
+      <c r="E9" s="187"/>
+      <c r="F9" s="187"/>
+      <c r="G9" s="188"/>
     </row>
     <row r="10" spans="1:17" ht="12" thickBot="1">
-      <c r="B10" s="189"/>
-      <c r="C10" s="190"/>
-      <c r="D10" s="190"/>
-      <c r="E10" s="190"/>
-      <c r="F10" s="190"/>
-      <c r="G10" s="191"/>
+      <c r="B10" s="190"/>
+      <c r="C10" s="191"/>
+      <c r="D10" s="191"/>
+      <c r="E10" s="191"/>
+      <c r="F10" s="191"/>
+      <c r="G10" s="192"/>
     </row>
     <row r="12" spans="1:17" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -8406,7 +8417,7 @@
         <v>114</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>125</v>
+        <v>186</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>3</v>
@@ -8581,10 +8592,10 @@
       <c r="B27" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="178" t="s">
+      <c r="C27" s="179" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="179"/>
+      <c r="D27" s="180"/>
       <c r="E27" s="34" t="s">
         <v>33</v>
       </c>
@@ -8602,10 +8613,10 @@
       <c r="B28" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="192" t="s">
+      <c r="C28" s="193" t="s">
         <v>113</v>
       </c>
-      <c r="D28" s="193"/>
+      <c r="D28" s="194"/>
       <c r="E28" s="46" t="s">
         <v>3</v>
       </c>
@@ -8621,8 +8632,8 @@
         <v>2</v>
       </c>
       <c r="B29" s="51"/>
-      <c r="C29" s="197"/>
-      <c r="D29" s="198"/>
+      <c r="C29" s="198"/>
+      <c r="D29" s="199"/>
       <c r="E29" s="52"/>
       <c r="F29" s="52"/>
       <c r="G29" s="53"/>
@@ -8632,8 +8643,8 @@
         <v>3</v>
       </c>
       <c r="B30" s="54"/>
-      <c r="C30" s="195"/>
-      <c r="D30" s="196"/>
+      <c r="C30" s="196"/>
+      <c r="D30" s="197"/>
       <c r="E30" s="58"/>
       <c r="F30" s="58"/>
       <c r="G30" s="55"/>
@@ -8650,14 +8661,14 @@
       <c r="B33" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="180" t="s">
+      <c r="C33" s="181" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="181"/>
-      <c r="E33" s="180" t="s">
+      <c r="D33" s="182"/>
+      <c r="E33" s="181" t="s">
         <v>36</v>
       </c>
-      <c r="F33" s="194"/>
+      <c r="F33" s="195"/>
       <c r="G33" s="38" t="s">
         <v>38</v>
       </c>
@@ -8667,16 +8678,16 @@
         <v>1</v>
       </c>
       <c r="B34" s="160" t="s">
-        <v>170</v>
-      </c>
-      <c r="C34" s="199" t="s">
+        <v>169</v>
+      </c>
+      <c r="C34" s="200" t="s">
         <v>113</v>
       </c>
-      <c r="D34" s="200"/>
-      <c r="E34" s="201" t="s">
+      <c r="D34" s="201"/>
+      <c r="E34" s="202" t="s">
         <v>142</v>
       </c>
-      <c r="F34" s="201"/>
+      <c r="F34" s="202"/>
       <c r="G34" s="161" t="s">
         <v>159</v>
       </c>
@@ -8686,16 +8697,16 @@
         <v>2</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="C35" s="202" t="s">
+        <v>162</v>
+      </c>
+      <c r="C35" s="203" t="s">
         <v>113</v>
       </c>
-      <c r="D35" s="203"/>
-      <c r="E35" s="204" t="s">
+      <c r="D35" s="204"/>
+      <c r="E35" s="205" t="s">
         <v>143</v>
       </c>
-      <c r="F35" s="204"/>
+      <c r="F35" s="205"/>
       <c r="G35" s="163" t="s">
         <v>159</v>
       </c>
@@ -8705,16 +8716,16 @@
         <v>3</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>179</v>
-      </c>
-      <c r="C36" s="207" t="s">
+        <v>178</v>
+      </c>
+      <c r="C36" s="208" t="s">
         <v>113</v>
       </c>
-      <c r="D36" s="208"/>
-      <c r="E36" s="205" t="s">
+      <c r="D36" s="209"/>
+      <c r="E36" s="206" t="s">
         <v>141</v>
       </c>
-      <c r="F36" s="206"/>
+      <c r="F36" s="207"/>
       <c r="G36" s="162" t="s">
         <v>159</v>
       </c>
@@ -8731,14 +8742,14 @@
       <c r="B39" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C39" s="180" t="s">
+      <c r="C39" s="181" t="s">
         <v>44</v>
       </c>
-      <c r="D39" s="181"/>
-      <c r="E39" s="180" t="s">
+      <c r="D39" s="182"/>
+      <c r="E39" s="181" t="s">
         <v>37</v>
       </c>
-      <c r="F39" s="194"/>
+      <c r="F39" s="195"/>
       <c r="G39" s="38" t="s">
         <v>39</v>
       </c>
@@ -8798,7 +8809,9 @@
   </sheetPr>
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
   <cols>
@@ -8828,103 +8841,105 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="171" t="s">
+      <c r="C2" s="172" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="172"/>
+      <c r="D2" s="173"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="171" t="s">
+      <c r="F2" s="172" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="175"/>
+      <c r="G2" s="176"/>
     </row>
     <row r="3" spans="1:16" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="173"/>
-      <c r="D3" s="174"/>
+      <c r="C3" s="174"/>
+      <c r="D3" s="175"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="176" t="s">
+      <c r="F3" s="177" t="s">
         <v>120</v>
       </c>
-      <c r="G3" s="177"/>
+      <c r="G3" s="178"/>
     </row>
     <row r="4" spans="1:16" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="173" t="s">
+      <c r="C4" s="174" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="174"/>
+      <c r="D4" s="175"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="173"/>
-      <c r="G4" s="177"/>
+      <c r="F4" s="174" t="s">
+        <v>187</v>
+      </c>
+      <c r="G4" s="178"/>
     </row>
     <row r="5" spans="1:16" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="173" t="s">
+      <c r="C5" s="174" t="s">
         <v>138</v>
       </c>
-      <c r="D5" s="174"/>
+      <c r="D5" s="175"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="173"/>
-      <c r="G5" s="177"/>
+      <c r="F5" s="174"/>
+      <c r="G5" s="178"/>
     </row>
     <row r="6" spans="1:16" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="173" t="s">
+      <c r="C6" s="174" t="s">
         <v>143</v>
       </c>
-      <c r="D6" s="174"/>
+      <c r="D6" s="175"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="173"/>
-      <c r="G6" s="177"/>
+      <c r="F6" s="174"/>
+      <c r="G6" s="178"/>
     </row>
     <row r="7" spans="1:16" ht="13">
-      <c r="B7" s="182" t="s">
+      <c r="B7" s="183" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="183"/>
-      <c r="D7" s="183"/>
-      <c r="E7" s="183"/>
-      <c r="F7" s="183"/>
-      <c r="G7" s="184"/>
+      <c r="C7" s="184"/>
+      <c r="D7" s="184"/>
+      <c r="E7" s="184"/>
+      <c r="F7" s="184"/>
+      <c r="G7" s="185"/>
     </row>
     <row r="8" spans="1:16">
-      <c r="B8" s="185"/>
-      <c r="C8" s="186"/>
-      <c r="D8" s="186"/>
-      <c r="E8" s="186"/>
-      <c r="F8" s="186"/>
-      <c r="G8" s="187"/>
+      <c r="B8" s="186"/>
+      <c r="C8" s="187"/>
+      <c r="D8" s="187"/>
+      <c r="E8" s="187"/>
+      <c r="F8" s="187"/>
+      <c r="G8" s="188"/>
     </row>
     <row r="9" spans="1:16">
-      <c r="B9" s="188"/>
-      <c r="C9" s="186"/>
-      <c r="D9" s="186"/>
-      <c r="E9" s="186"/>
-      <c r="F9" s="186"/>
-      <c r="G9" s="187"/>
+      <c r="B9" s="189"/>
+      <c r="C9" s="187"/>
+      <c r="D9" s="187"/>
+      <c r="E9" s="187"/>
+      <c r="F9" s="187"/>
+      <c r="G9" s="188"/>
     </row>
     <row r="10" spans="1:16" ht="12" thickBot="1">
-      <c r="B10" s="189"/>
-      <c r="C10" s="190"/>
-      <c r="D10" s="190"/>
-      <c r="E10" s="190"/>
-      <c r="F10" s="190"/>
-      <c r="G10" s="191"/>
+      <c r="B10" s="190"/>
+      <c r="C10" s="191"/>
+      <c r="D10" s="191"/>
+      <c r="E10" s="191"/>
+      <c r="F10" s="191"/>
+      <c r="G10" s="192"/>
     </row>
     <row r="12" spans="1:16" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -8960,10 +8975,10 @@
         <v>113</v>
       </c>
       <c r="J13" s="128" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K13" s="128" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L13" s="128"/>
       <c r="M13" s="128" t="s">
@@ -8986,7 +9001,7 @@
       <c r="B14" s="63" t="s">
         <v>156</v>
       </c>
-      <c r="C14" s="64" t="s">
+      <c r="C14" s="65" t="s">
         <v>113</v>
       </c>
       <c r="D14" s="65" t="s">
@@ -9004,12 +9019,12 @@
         <v>1</v>
       </c>
       <c r="J14" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="K14" s="221" t="s">
         <v>172</v>
       </c>
-      <c r="K14" s="220" t="s">
-        <v>173</v>
-      </c>
-      <c r="L14" s="220"/>
+      <c r="L14" s="221"/>
       <c r="M14" s="127" t="s">
         <v>155</v>
       </c>
@@ -9032,27 +9047,25 @@
         <v>157</v>
       </c>
       <c r="C15" s="65" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F15" s="67"/>
-      <c r="G15" s="107" t="s">
-        <v>109</v>
-      </c>
+      <c r="G15" s="107"/>
       <c r="H15" s="87"/>
       <c r="I15" s="13">
         <v>2</v>
       </c>
       <c r="J15" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="K15" s="13" t="s">
         <v>174</v>
-      </c>
-      <c r="K15" s="13" t="s">
-        <v>175</v>
       </c>
       <c r="M15" s="127" t="s">
         <v>155</v>
@@ -9076,18 +9089,16 @@
         <v>12</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>161</v>
+        <v>185</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="67"/>
-      <c r="G16" s="117" t="s">
-        <v>126</v>
-      </c>
+      <c r="G16" s="117"/>
       <c r="H16" s="87"/>
     </row>
     <row r="17" spans="1:7">
@@ -9236,10 +9247,10 @@
       <c r="B27" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="178" t="s">
+      <c r="C27" s="179" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="179"/>
+      <c r="D27" s="180"/>
       <c r="E27" s="34" t="s">
         <v>33</v>
       </c>
@@ -9257,10 +9268,10 @@
       <c r="B28" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="192" t="s">
+      <c r="C28" s="193" t="s">
         <v>113</v>
       </c>
-      <c r="D28" s="193"/>
+      <c r="D28" s="194"/>
       <c r="E28" s="46" t="s">
         <v>3</v>
       </c>
@@ -9274,8 +9285,8 @@
         <v>2</v>
       </c>
       <c r="B29" s="51"/>
-      <c r="C29" s="197"/>
-      <c r="D29" s="198"/>
+      <c r="C29" s="198"/>
+      <c r="D29" s="199"/>
       <c r="E29" s="52"/>
       <c r="F29" s="52"/>
       <c r="G29" s="53"/>
@@ -9285,8 +9296,8 @@
         <v>3</v>
       </c>
       <c r="B30" s="54"/>
-      <c r="C30" s="195"/>
-      <c r="D30" s="196"/>
+      <c r="C30" s="196"/>
+      <c r="D30" s="197"/>
       <c r="E30" s="58"/>
       <c r="F30" s="58"/>
       <c r="G30" s="55"/>
@@ -9303,14 +9314,14 @@
       <c r="B33" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="180" t="s">
+      <c r="C33" s="181" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="181"/>
-      <c r="E33" s="180" t="s">
+      <c r="D33" s="182"/>
+      <c r="E33" s="181" t="s">
         <v>36</v>
       </c>
-      <c r="F33" s="194"/>
+      <c r="F33" s="195"/>
       <c r="G33" s="38" t="s">
         <v>38</v>
       </c>
@@ -9320,27 +9331,27 @@
         <v>1</v>
       </c>
       <c r="B34" s="51" t="s">
+        <v>163</v>
+      </c>
+      <c r="C34" s="214" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" s="215"/>
+      <c r="E34" s="216" t="s">
+        <v>142</v>
+      </c>
+      <c r="F34" s="217"/>
+      <c r="G34" s="155" t="s">
         <v>164</v>
-      </c>
-      <c r="C34" s="213" t="s">
-        <v>113</v>
-      </c>
-      <c r="D34" s="214"/>
-      <c r="E34" s="215" t="s">
-        <v>142</v>
-      </c>
-      <c r="F34" s="216"/>
-      <c r="G34" s="155" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="13">
       <c r="A35" s="153"/>
       <c r="B35" s="154"/>
-      <c r="C35" s="217"/>
-      <c r="D35" s="218"/>
-      <c r="E35" s="219"/>
-      <c r="F35" s="219"/>
+      <c r="C35" s="218"/>
+      <c r="D35" s="219"/>
+      <c r="E35" s="220"/>
+      <c r="F35" s="220"/>
       <c r="G35" s="154"/>
     </row>
     <row r="37" spans="1:7" ht="12" thickBot="1">
@@ -9355,14 +9366,14 @@
       <c r="B38" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="180" t="s">
+      <c r="C38" s="181" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="181"/>
-      <c r="E38" s="180" t="s">
+      <c r="D38" s="182"/>
+      <c r="E38" s="181" t="s">
         <v>37</v>
       </c>
-      <c r="F38" s="181"/>
+      <c r="F38" s="182"/>
       <c r="G38" s="38" t="s">
         <v>39</v>
       </c>
@@ -9372,16 +9383,16 @@
         <v>1</v>
       </c>
       <c r="B39" s="157" t="s">
-        <v>163</v>
-      </c>
-      <c r="C39" s="209" t="s">
+        <v>162</v>
+      </c>
+      <c r="C39" s="210" t="s">
         <v>160</v>
       </c>
-      <c r="D39" s="210"/>
-      <c r="E39" s="211" t="s">
+      <c r="D39" s="211"/>
+      <c r="E39" s="212" t="s">
         <v>106</v>
       </c>
-      <c r="F39" s="212"/>
+      <c r="F39" s="213"/>
       <c r="G39" s="158" t="s">
         <v>113</v>
       </c>
@@ -9453,8 +9464,8 @@
   </sheetPr>
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -9485,103 +9496,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="171" t="s">
+      <c r="C2" s="172" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="172"/>
+      <c r="D2" s="173"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="171" t="s">
+      <c r="F2" s="172" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="175"/>
+      <c r="G2" s="176"/>
     </row>
     <row r="3" spans="1:15" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="173"/>
-      <c r="D3" s="174"/>
+      <c r="C3" s="174"/>
+      <c r="D3" s="175"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="176" t="s">
+      <c r="F3" s="177" t="s">
         <v>120</v>
       </c>
-      <c r="G3" s="177"/>
+      <c r="G3" s="178"/>
     </row>
     <row r="4" spans="1:15" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="173" t="s">
+      <c r="C4" s="174" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="174"/>
+      <c r="D4" s="175"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="173"/>
-      <c r="G4" s="177"/>
+      <c r="F4" s="174"/>
+      <c r="G4" s="178"/>
     </row>
     <row r="5" spans="1:15" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="173" t="s">
+      <c r="C5" s="174" t="s">
         <v>139</v>
       </c>
-      <c r="D5" s="174"/>
+      <c r="D5" s="175"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="173"/>
-      <c r="G5" s="177"/>
+      <c r="F5" s="174"/>
+      <c r="G5" s="178"/>
     </row>
     <row r="6" spans="1:15" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="173" t="s">
+      <c r="C6" s="174" t="s">
         <v>142</v>
       </c>
-      <c r="D6" s="174"/>
+      <c r="D6" s="175"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="173"/>
-      <c r="G6" s="177"/>
+      <c r="F6" s="174"/>
+      <c r="G6" s="178"/>
     </row>
     <row r="7" spans="1:15" ht="13">
-      <c r="B7" s="182" t="s">
+      <c r="B7" s="183" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="183"/>
-      <c r="D7" s="183"/>
-      <c r="E7" s="183"/>
-      <c r="F7" s="183"/>
-      <c r="G7" s="184"/>
+      <c r="C7" s="184"/>
+      <c r="D7" s="184"/>
+      <c r="E7" s="184"/>
+      <c r="F7" s="184"/>
+      <c r="G7" s="185"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="B8" s="185"/>
-      <c r="C8" s="186"/>
-      <c r="D8" s="186"/>
-      <c r="E8" s="186"/>
-      <c r="F8" s="186"/>
-      <c r="G8" s="187"/>
+      <c r="B8" s="186"/>
+      <c r="C8" s="187"/>
+      <c r="D8" s="187"/>
+      <c r="E8" s="187"/>
+      <c r="F8" s="187"/>
+      <c r="G8" s="188"/>
     </row>
     <row r="9" spans="1:15">
-      <c r="B9" s="188"/>
-      <c r="C9" s="186"/>
-      <c r="D9" s="186"/>
-      <c r="E9" s="186"/>
-      <c r="F9" s="186"/>
-      <c r="G9" s="187"/>
+      <c r="B9" s="189"/>
+      <c r="C9" s="187"/>
+      <c r="D9" s="187"/>
+      <c r="E9" s="187"/>
+      <c r="F9" s="187"/>
+      <c r="G9" s="188"/>
     </row>
     <row r="10" spans="1:15" ht="12" thickBot="1">
-      <c r="B10" s="189"/>
-      <c r="C10" s="190"/>
-      <c r="D10" s="190"/>
-      <c r="E10" s="190"/>
-      <c r="F10" s="190"/>
-      <c r="G10" s="191"/>
+      <c r="B10" s="190"/>
+      <c r="C10" s="191"/>
+      <c r="D10" s="191"/>
+      <c r="E10" s="191"/>
+      <c r="F10" s="191"/>
+      <c r="G10" s="192"/>
     </row>
     <row r="12" spans="1:15" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -9617,7 +9628,7 @@
         <v>113</v>
       </c>
       <c r="J13" s="128" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K13" s="128" t="s">
         <v>100</v>
@@ -9629,7 +9640,7 @@
         <v>6</v>
       </c>
       <c r="N13" s="128" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O13" s="128" t="s">
         <v>159</v>
@@ -9640,9 +9651,9 @@
         <v>1</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>166</v>
-      </c>
-      <c r="C14" s="64" t="s">
+        <v>165</v>
+      </c>
+      <c r="C14" s="65" t="s">
         <v>113</v>
       </c>
       <c r="D14" s="65" t="s">
@@ -9660,7 +9671,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K14" s="127">
         <v>41922.465277777781</v>
@@ -9687,24 +9698,22 @@
         <v>12</v>
       </c>
       <c r="C15" s="65" t="s">
+        <v>166</v>
+      </c>
+      <c r="D15" s="65" t="s">
         <v>167</v>
-      </c>
-      <c r="D15" s="65" t="s">
-        <v>168</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F15" s="67"/>
-      <c r="G15" s="107" t="s">
-        <v>109</v>
-      </c>
+      <c r="G15" s="107"/>
       <c r="H15" s="87"/>
       <c r="I15" s="13">
         <v>2</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K15" s="127">
         <v>41922.46875</v>
@@ -9774,7 +9783,7 @@
         <v>156</v>
       </c>
       <c r="C18" s="138" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D18" s="138" t="s">
         <v>53</v>
@@ -9877,10 +9886,10 @@
       <c r="B27" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="178" t="s">
+      <c r="C27" s="179" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="179"/>
+      <c r="D27" s="180"/>
       <c r="E27" s="34" t="s">
         <v>33</v>
       </c>
@@ -9898,10 +9907,10 @@
       <c r="B28" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="192" t="s">
+      <c r="C28" s="193" t="s">
         <v>113</v>
       </c>
-      <c r="D28" s="193"/>
+      <c r="D28" s="194"/>
       <c r="E28" s="46" t="s">
         <v>3</v>
       </c>
@@ -9909,7 +9918,7 @@
         <v>3</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="13" customHeight="1">
@@ -9917,8 +9926,8 @@
         <v>2</v>
       </c>
       <c r="B29" s="51"/>
-      <c r="C29" s="197"/>
-      <c r="D29" s="198"/>
+      <c r="C29" s="198"/>
+      <c r="D29" s="199"/>
       <c r="E29" s="52"/>
       <c r="F29" s="52"/>
       <c r="G29" s="53"/>
@@ -9928,8 +9937,8 @@
         <v>3</v>
       </c>
       <c r="B30" s="54"/>
-      <c r="C30" s="195"/>
-      <c r="D30" s="196"/>
+      <c r="C30" s="196"/>
+      <c r="D30" s="197"/>
       <c r="E30" s="58"/>
       <c r="F30" s="58"/>
       <c r="G30" s="55"/>
@@ -9946,14 +9955,14 @@
       <c r="B33" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="180" t="s">
+      <c r="C33" s="181" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="181"/>
-      <c r="E33" s="180" t="s">
+      <c r="D33" s="182"/>
+      <c r="E33" s="181" t="s">
         <v>36</v>
       </c>
-      <c r="F33" s="194"/>
+      <c r="F33" s="195"/>
       <c r="G33" s="38" t="s">
         <v>38</v>
       </c>
@@ -9970,14 +9979,14 @@
       <c r="B36" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="180" t="s">
+      <c r="C36" s="181" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="181"/>
-      <c r="E36" s="180" t="s">
+      <c r="D36" s="182"/>
+      <c r="E36" s="181" t="s">
         <v>37</v>
       </c>
-      <c r="F36" s="194"/>
+      <c r="F36" s="195"/>
       <c r="G36" s="38" t="s">
         <v>39</v>
       </c>
@@ -9987,16 +9996,16 @@
         <v>1</v>
       </c>
       <c r="B37" s="160" t="s">
+        <v>163</v>
+      </c>
+      <c r="C37" s="200" t="s">
         <v>164</v>
       </c>
-      <c r="C37" s="199" t="s">
-        <v>165</v>
-      </c>
-      <c r="D37" s="200"/>
-      <c r="E37" s="201" t="s">
+      <c r="D37" s="201"/>
+      <c r="E37" s="202" t="s">
         <v>143</v>
       </c>
-      <c r="F37" s="201"/>
+      <c r="F37" s="202"/>
       <c r="G37" s="161" t="s">
         <v>113</v>
       </c>
@@ -10006,16 +10015,16 @@
         <v>2</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="C38" s="221" t="s">
+        <v>169</v>
+      </c>
+      <c r="C38" s="222" t="s">
         <v>159</v>
       </c>
-      <c r="D38" s="222"/>
-      <c r="E38" s="223" t="s">
+      <c r="D38" s="223"/>
+      <c r="E38" s="224" t="s">
         <v>106</v>
       </c>
-      <c r="F38" s="223"/>
+      <c r="F38" s="224"/>
       <c r="G38" s="162" t="s">
         <v>113</v>
       </c>
@@ -10068,8 +10077,8 @@
   </sheetPr>
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -10101,103 +10110,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="171" t="s">
+      <c r="C2" s="172" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="172"/>
+      <c r="D2" s="173"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="171" t="s">
+      <c r="F2" s="172" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="175"/>
+      <c r="G2" s="176"/>
     </row>
     <row r="3" spans="1:13" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="173"/>
-      <c r="D3" s="174"/>
+      <c r="C3" s="174"/>
+      <c r="D3" s="175"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="176" t="s">
+      <c r="F3" s="177" t="s">
         <v>120</v>
       </c>
-      <c r="G3" s="177"/>
+      <c r="G3" s="178"/>
     </row>
     <row r="4" spans="1:13" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="173" t="s">
+      <c r="C4" s="174" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="174"/>
+      <c r="D4" s="175"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="173"/>
-      <c r="G4" s="177"/>
+      <c r="F4" s="174"/>
+      <c r="G4" s="178"/>
     </row>
     <row r="5" spans="1:13" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="173" t="s">
+      <c r="C5" s="174" t="s">
         <v>140</v>
       </c>
-      <c r="D5" s="174"/>
+      <c r="D5" s="175"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="173"/>
-      <c r="G5" s="177"/>
+      <c r="F5" s="174"/>
+      <c r="G5" s="178"/>
     </row>
     <row r="6" spans="1:13" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="173" t="s">
+      <c r="C6" s="174" t="s">
         <v>141</v>
       </c>
-      <c r="D6" s="174"/>
+      <c r="D6" s="175"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="173"/>
-      <c r="G6" s="177"/>
+      <c r="F6" s="174"/>
+      <c r="G6" s="178"/>
     </row>
     <row r="7" spans="1:13" ht="13">
-      <c r="B7" s="182" t="s">
+      <c r="B7" s="183" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="183"/>
-      <c r="D7" s="183"/>
-      <c r="E7" s="183"/>
-      <c r="F7" s="183"/>
-      <c r="G7" s="184"/>
+      <c r="C7" s="184"/>
+      <c r="D7" s="184"/>
+      <c r="E7" s="184"/>
+      <c r="F7" s="184"/>
+      <c r="G7" s="185"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="B8" s="185"/>
-      <c r="C8" s="186"/>
-      <c r="D8" s="186"/>
-      <c r="E8" s="186"/>
-      <c r="F8" s="186"/>
-      <c r="G8" s="187"/>
+      <c r="B8" s="186"/>
+      <c r="C8" s="187"/>
+      <c r="D8" s="187"/>
+      <c r="E8" s="187"/>
+      <c r="F8" s="187"/>
+      <c r="G8" s="188"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="B9" s="188"/>
-      <c r="C9" s="186"/>
-      <c r="D9" s="186"/>
-      <c r="E9" s="186"/>
-      <c r="F9" s="186"/>
-      <c r="G9" s="187"/>
+      <c r="B9" s="189"/>
+      <c r="C9" s="187"/>
+      <c r="D9" s="187"/>
+      <c r="E9" s="187"/>
+      <c r="F9" s="187"/>
+      <c r="G9" s="188"/>
     </row>
     <row r="10" spans="1:13" ht="12" thickBot="1">
-      <c r="B10" s="189"/>
-      <c r="C10" s="190"/>
-      <c r="D10" s="190"/>
-      <c r="E10" s="190"/>
-      <c r="F10" s="190"/>
-      <c r="G10" s="191"/>
+      <c r="B10" s="190"/>
+      <c r="C10" s="191"/>
+      <c r="D10" s="191"/>
+      <c r="E10" s="191"/>
+      <c r="F10" s="191"/>
+      <c r="G10" s="192"/>
     </row>
     <row r="12" spans="1:13" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -10233,13 +10242,13 @@
         <v>113</v>
       </c>
       <c r="J13" s="128" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K13" s="128" t="s">
         <v>100</v>
       </c>
       <c r="L13" s="128" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M13" s="128" t="s">
         <v>159</v>
@@ -10250,9 +10259,9 @@
         <v>1</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>178</v>
-      </c>
-      <c r="C14" s="64" t="s">
+        <v>177</v>
+      </c>
+      <c r="C14" s="65" t="s">
         <v>113</v>
       </c>
       <c r="D14" s="65" t="s">
@@ -10288,19 +10297,19 @@
         <v>2</v>
       </c>
       <c r="B15" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="C15" s="18" t="s">
         <v>183</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>184</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>125</v>
       </c>
       <c r="E15" s="165" t="s">
-        <v>185</v>
+        <v>3</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H15" s="87"/>
       <c r="I15" s="13">
@@ -10348,10 +10357,10 @@
         <v>4</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C17" s="65" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D17" s="65" t="s">
         <v>147</v>
@@ -10466,10 +10475,10 @@
       <c r="B27" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="178" t="s">
+      <c r="C27" s="179" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="179"/>
+      <c r="D27" s="180"/>
       <c r="E27" s="34" t="s">
         <v>33</v>
       </c>
@@ -10487,10 +10496,10 @@
       <c r="B28" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="192" t="s">
+      <c r="C28" s="193" t="s">
         <v>113</v>
       </c>
-      <c r="D28" s="193"/>
+      <c r="D28" s="194"/>
       <c r="E28" s="46" t="s">
         <v>3</v>
       </c>
@@ -10504,8 +10513,8 @@
         <v>2</v>
       </c>
       <c r="B29" s="51"/>
-      <c r="C29" s="197"/>
-      <c r="D29" s="198"/>
+      <c r="C29" s="198"/>
+      <c r="D29" s="199"/>
       <c r="E29" s="52"/>
       <c r="F29" s="52"/>
       <c r="G29" s="53"/>
@@ -10515,8 +10524,8 @@
         <v>3</v>
       </c>
       <c r="B30" s="54"/>
-      <c r="C30" s="195"/>
-      <c r="D30" s="196"/>
+      <c r="C30" s="196"/>
+      <c r="D30" s="197"/>
       <c r="E30" s="58"/>
       <c r="F30" s="58"/>
       <c r="G30" s="55"/>
@@ -10533,14 +10542,14 @@
       <c r="B33" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="180" t="s">
+      <c r="C33" s="181" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="181"/>
-      <c r="E33" s="180" t="s">
+      <c r="D33" s="182"/>
+      <c r="E33" s="181" t="s">
         <v>36</v>
       </c>
-      <c r="F33" s="194"/>
+      <c r="F33" s="195"/>
       <c r="G33" s="38" t="s">
         <v>38</v>
       </c>
@@ -10557,14 +10566,14 @@
       <c r="B36" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="180" t="s">
+      <c r="C36" s="181" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="181"/>
-      <c r="E36" s="180" t="s">
+      <c r="D36" s="182"/>
+      <c r="E36" s="181" t="s">
         <v>37</v>
       </c>
-      <c r="F36" s="194"/>
+      <c r="F36" s="195"/>
       <c r="G36" s="38" t="s">
         <v>39</v>
       </c>
@@ -10574,16 +10583,16 @@
         <v>1</v>
       </c>
       <c r="B37" s="166" t="s">
-        <v>179</v>
-      </c>
-      <c r="C37" s="224" t="s">
+        <v>178</v>
+      </c>
+      <c r="C37" s="225" t="s">
         <v>159</v>
       </c>
-      <c r="D37" s="225"/>
-      <c r="E37" s="226" t="s">
+      <c r="D37" s="226"/>
+      <c r="E37" s="227" t="s">
         <v>106</v>
       </c>
-      <c r="F37" s="226"/>
+      <c r="F37" s="227"/>
       <c r="G37" s="158" t="s">
         <v>113</v>
       </c>
@@ -10658,103 +10667,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="171" t="s">
+      <c r="C2" s="172" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="172"/>
+      <c r="D2" s="173"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="171" t="s">
+      <c r="F2" s="172" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="175"/>
+      <c r="G2" s="176"/>
     </row>
     <row r="3" spans="1:11" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="173"/>
-      <c r="D3" s="174"/>
+      <c r="C3" s="174"/>
+      <c r="D3" s="175"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="173" t="s">
+      <c r="F3" s="174" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="177"/>
+      <c r="G3" s="178"/>
     </row>
     <row r="4" spans="1:11" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="173" t="s">
+      <c r="C4" s="174" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="174"/>
+      <c r="D4" s="175"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="173"/>
-      <c r="G4" s="177"/>
+      <c r="F4" s="174"/>
+      <c r="G4" s="178"/>
     </row>
     <row r="5" spans="1:11" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="173" t="s">
+      <c r="C5" s="174" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="174"/>
+      <c r="D5" s="175"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="173"/>
-      <c r="G5" s="177"/>
+      <c r="F5" s="174"/>
+      <c r="G5" s="178"/>
     </row>
     <row r="6" spans="1:11" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="173" t="s">
+      <c r="C6" s="174" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="174"/>
+      <c r="D6" s="175"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="173"/>
-      <c r="G6" s="177"/>
+      <c r="F6" s="174"/>
+      <c r="G6" s="178"/>
     </row>
     <row r="7" spans="1:11" ht="13">
-      <c r="B7" s="182" t="s">
+      <c r="B7" s="183" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="183"/>
-      <c r="D7" s="183"/>
-      <c r="E7" s="183"/>
-      <c r="F7" s="183"/>
-      <c r="G7" s="184"/>
+      <c r="C7" s="184"/>
+      <c r="D7" s="184"/>
+      <c r="E7" s="184"/>
+      <c r="F7" s="184"/>
+      <c r="G7" s="185"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="B8" s="185"/>
-      <c r="C8" s="186"/>
-      <c r="D8" s="186"/>
-      <c r="E8" s="186"/>
-      <c r="F8" s="186"/>
-      <c r="G8" s="187"/>
+      <c r="B8" s="186"/>
+      <c r="C8" s="187"/>
+      <c r="D8" s="187"/>
+      <c r="E8" s="187"/>
+      <c r="F8" s="187"/>
+      <c r="G8" s="188"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="B9" s="188"/>
-      <c r="C9" s="186"/>
-      <c r="D9" s="186"/>
-      <c r="E9" s="186"/>
-      <c r="F9" s="186"/>
-      <c r="G9" s="187"/>
+      <c r="B9" s="189"/>
+      <c r="C9" s="187"/>
+      <c r="D9" s="187"/>
+      <c r="E9" s="187"/>
+      <c r="F9" s="187"/>
+      <c r="G9" s="188"/>
     </row>
     <row r="10" spans="1:11" ht="12" thickBot="1">
-      <c r="B10" s="189"/>
-      <c r="C10" s="190"/>
-      <c r="D10" s="190"/>
-      <c r="E10" s="190"/>
-      <c r="F10" s="190"/>
-      <c r="G10" s="191"/>
+      <c r="B10" s="190"/>
+      <c r="C10" s="191"/>
+      <c r="D10" s="191"/>
+      <c r="E10" s="191"/>
+      <c r="F10" s="191"/>
+      <c r="G10" s="192"/>
     </row>
     <row r="12" spans="1:11" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -10976,10 +10985,10 @@
       <c r="B24" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="178" t="s">
+      <c r="C24" s="179" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="179"/>
+      <c r="D24" s="180"/>
       <c r="E24" s="34" t="s">
         <v>33</v>
       </c>
@@ -10997,10 +11006,10 @@
       <c r="B25" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="192" t="s">
+      <c r="C25" s="193" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="193"/>
+      <c r="D25" s="194"/>
       <c r="E25" s="46" t="s">
         <v>3</v>
       </c>
@@ -11014,10 +11023,10 @@
         <v>2</v>
       </c>
       <c r="B26" s="54"/>
-      <c r="C26" s="207" t="s">
+      <c r="C26" s="208" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="208"/>
+      <c r="D26" s="209"/>
       <c r="E26" s="58"/>
       <c r="F26" s="58" t="s">
         <v>3</v>
@@ -11036,14 +11045,14 @@
       <c r="B29" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="180" t="s">
+      <c r="C29" s="181" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="181"/>
-      <c r="E29" s="180" t="s">
+      <c r="D29" s="182"/>
+      <c r="E29" s="181" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="194"/>
+      <c r="F29" s="195"/>
       <c r="G29" s="38" t="s">
         <v>38</v>
       </c>
@@ -11060,14 +11069,14 @@
       <c r="B32" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="180" t="s">
+      <c r="C32" s="181" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="181"/>
-      <c r="E32" s="180" t="s">
+      <c r="D32" s="182"/>
+      <c r="E32" s="181" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="194"/>
+      <c r="F32" s="195"/>
       <c r="G32" s="38" t="s">
         <v>39</v>
       </c>
@@ -11077,14 +11086,14 @@
         <v>1</v>
       </c>
       <c r="B33" s="26"/>
-      <c r="C33" s="227" t="s">
+      <c r="C33" s="228" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="228"/>
-      <c r="E33" s="207" t="s">
+      <c r="D33" s="229"/>
+      <c r="E33" s="208" t="s">
         <v>47</v>
       </c>
-      <c r="F33" s="208"/>
+      <c r="F33" s="209"/>
       <c r="G33" s="28" t="s">
         <v>49</v>
       </c>
@@ -11159,105 +11168,105 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="171" t="s">
+      <c r="C2" s="172" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="172"/>
+      <c r="D2" s="173"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="171" t="s">
+      <c r="F2" s="172" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="175"/>
+      <c r="G2" s="176"/>
     </row>
     <row r="3" spans="1:7" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="173"/>
-      <c r="D3" s="174"/>
+      <c r="C3" s="174"/>
+      <c r="D3" s="175"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="173" t="s">
+      <c r="F3" s="174" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="177"/>
+      <c r="G3" s="178"/>
     </row>
     <row r="4" spans="1:7" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="173" t="s">
+      <c r="C4" s="174" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="174"/>
+      <c r="D4" s="175"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="173"/>
-      <c r="G4" s="177"/>
+      <c r="F4" s="174"/>
+      <c r="G4" s="178"/>
     </row>
     <row r="5" spans="1:7" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="173" t="s">
+      <c r="C5" s="174" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="174"/>
+      <c r="D5" s="175"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="173"/>
-      <c r="G5" s="177"/>
+      <c r="F5" s="174"/>
+      <c r="G5" s="178"/>
     </row>
     <row r="6" spans="1:7" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="173" t="s">
+      <c r="C6" s="174" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="174"/>
+      <c r="D6" s="175"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="173"/>
-      <c r="G6" s="177"/>
+      <c r="F6" s="174"/>
+      <c r="G6" s="178"/>
     </row>
     <row r="7" spans="1:7" ht="13">
-      <c r="B7" s="182" t="s">
+      <c r="B7" s="183" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="183"/>
-      <c r="D7" s="183"/>
-      <c r="E7" s="183"/>
-      <c r="F7" s="183"/>
-      <c r="G7" s="184"/>
+      <c r="C7" s="184"/>
+      <c r="D7" s="184"/>
+      <c r="E7" s="184"/>
+      <c r="F7" s="184"/>
+      <c r="G7" s="185"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="B8" s="185" t="s">
+      <c r="B8" s="186" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="186"/>
-      <c r="D8" s="186"/>
-      <c r="E8" s="186"/>
-      <c r="F8" s="186"/>
-      <c r="G8" s="187"/>
+      <c r="C8" s="187"/>
+      <c r="D8" s="187"/>
+      <c r="E8" s="187"/>
+      <c r="F8" s="187"/>
+      <c r="G8" s="188"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="B9" s="188"/>
-      <c r="C9" s="186"/>
-      <c r="D9" s="186"/>
-      <c r="E9" s="186"/>
-      <c r="F9" s="186"/>
-      <c r="G9" s="187"/>
+      <c r="B9" s="189"/>
+      <c r="C9" s="187"/>
+      <c r="D9" s="187"/>
+      <c r="E9" s="187"/>
+      <c r="F9" s="187"/>
+      <c r="G9" s="188"/>
     </row>
     <row r="10" spans="1:7" ht="12" thickBot="1">
-      <c r="B10" s="189"/>
-      <c r="C10" s="190"/>
-      <c r="D10" s="190"/>
-      <c r="E10" s="190"/>
-      <c r="F10" s="190"/>
-      <c r="G10" s="191"/>
+      <c r="B10" s="190"/>
+      <c r="C10" s="191"/>
+      <c r="D10" s="191"/>
+      <c r="E10" s="191"/>
+      <c r="F10" s="191"/>
+      <c r="G10" s="192"/>
     </row>
     <row r="12" spans="1:7" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -11362,10 +11371,10 @@
       <c r="B19" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="178" t="s">
+      <c r="C19" s="179" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="179"/>
+      <c r="D19" s="180"/>
       <c r="E19" s="34" t="s">
         <v>33</v>
       </c>
@@ -11383,10 +11392,10 @@
       <c r="B20" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="192" t="s">
+      <c r="C20" s="193" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="193"/>
+      <c r="D20" s="194"/>
       <c r="E20" s="46" t="s">
         <v>3</v>
       </c>
@@ -11400,10 +11409,10 @@
         <v>2</v>
       </c>
       <c r="B21" s="26"/>
-      <c r="C21" s="227" t="s">
+      <c r="C21" s="228" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="228"/>
+      <c r="D21" s="229"/>
       <c r="E21" s="45"/>
       <c r="F21" s="45" t="s">
         <v>3</v>
@@ -11422,14 +11431,14 @@
       <c r="B24" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="180" t="s">
+      <c r="C24" s="181" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="181"/>
-      <c r="E24" s="180" t="s">
+      <c r="D24" s="182"/>
+      <c r="E24" s="181" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="194"/>
+      <c r="F24" s="195"/>
       <c r="G24" s="38" t="s">
         <v>38</v>
       </c>
@@ -11446,14 +11455,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="180" t="s">
+      <c r="C27" s="181" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="181"/>
-      <c r="E27" s="180" t="s">
+      <c r="D27" s="182"/>
+      <c r="E27" s="181" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="194"/>
+      <c r="F27" s="195"/>
       <c r="G27" s="38" t="s">
         <v>39</v>
       </c>
@@ -11463,10 +11472,10 @@
         <v>1</v>
       </c>
       <c r="B28" s="26"/>
-      <c r="C28" s="227"/>
-      <c r="D28" s="228"/>
-      <c r="E28" s="207"/>
-      <c r="F28" s="208"/>
+      <c r="C28" s="228"/>
+      <c r="D28" s="229"/>
+      <c r="E28" s="208"/>
+      <c r="F28" s="209"/>
       <c r="G28" s="28"/>
     </row>
   </sheetData>

</xml_diff>